<commit_message>
changes after code review
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_GROCERY.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_GROCERY.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="151">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -449,9 +449,6 @@
   </si>
   <si>
     <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manufacturer_except</t>
   </si>
   <si>
     <t xml:space="preserve">KO PRODUCT</t>
@@ -760,14 +757,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="1020" min="7" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="1020" min="7" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,10 +1020,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,24 +1084,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="76.0511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="84.7906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.5116279069767"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="78.2697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.98139534883721"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="87.2511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1440,22 +1437,21 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.306976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,23 +1718,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.711627906977"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.3813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.0604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="117.153488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.1953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.2418604651163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.306976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,17 +2097,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,32 +2188,32 @@
   </sheetPr>
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.506976744186"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="77.2837209302326"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.6093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.4604651162791"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="79.6232558139535"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,16 +2649,16 @@
         <v>102</v>
       </c>
       <c r="G13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K13" s="12" t="n">
         <v>2</v>
@@ -2677,7 +2673,7 @@
         <v>16</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2681,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>138</v>
@@ -2697,19 +2693,19 @@
         <v>140</v>
       </c>
       <c r="F14" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="I14" s="0" t="s">
+      <c r="J14" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>147</v>
       </c>
       <c r="K14" s="12" t="n">
         <v>2</v>
@@ -2724,7 +2720,7 @@
         <v>16</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2732,7 +2728,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>138</v>
@@ -2744,19 +2740,19 @@
         <v>140</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K15" s="12" t="n">
         <v>2</v>
@@ -2771,7 +2767,7 @@
         <v>16</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,7 +2775,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>138</v>
@@ -2794,16 +2790,16 @@
         <v>104</v>
       </c>
       <c r="G16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K16" s="12" t="n">
         <v>2</v>
@@ -2818,7 +2814,7 @@
         <v>16</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,7 +2822,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>138</v>
@@ -2841,16 +2837,16 @@
         <v>113</v>
       </c>
       <c r="G17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2</v>
@@ -2865,7 +2861,7 @@
         <v>16</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,7 +2869,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>138</v>
@@ -2888,13 +2884,13 @@
         <v>108</v>
       </c>
       <c r="G18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="H18" s="0" t="s">
-        <v>142</v>
-      </c>
       <c r="I18" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>106</v>
@@ -2912,7 +2908,7 @@
         <v>16</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
changes to grocery template
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_GROCERY.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_GROCERY.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$16</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$16</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$S$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$S$16</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +52,7 @@
     <t xml:space="preserve">Bonus</t>
   </si>
   <si>
-    <t xml:space="preserve">Grocery</t>
+    <t xml:space="preserve">GROCERY</t>
   </si>
   <si>
     <t xml:space="preserve">COOLER</t>
@@ -855,21 +856,21 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,15 +1160,15 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,29 +1224,29 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.8511627906977"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="80.6046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="89.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.3116279069767"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="83.0651162790698"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="92.5441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,7 +1335,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
         <v>19</v>
       </c>
@@ -1576,7 +1577,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
@@ -1664,22 +1665,22 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.3627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="54.6418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,7 +1769,7 @@
       <c r="I3" s="15"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -1792,7 +1793,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
@@ -1816,7 +1817,7 @@
       </c>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
@@ -1840,7 +1841,7 @@
       </c>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>26</v>
       </c>
@@ -1888,7 +1889,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>28</v>
       </c>
@@ -1912,7 +1913,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>28</v>
       </c>
@@ -1936,7 +1937,7 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>28</v>
       </c>
@@ -1960,7 +1961,7 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -2003,29 +2004,29 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.6093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2279069767442"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2088,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
@@ -2385,22 +2386,22 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,33 +2482,33 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="101.032558139535"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.5302325581395"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.1813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.1953488372093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.01395348837209"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.246511627907"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="81.9581395348837"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.5441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="103.986046511628"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="88.1116279069768"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.1627906976744"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0604651162791"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="84.4186046511628"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2569,7 +2570,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="13" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
         <v>16</v>
       </c>
@@ -2713,7 +2714,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
@@ -2746,7 +2747,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -2827,7 +2828,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
@@ -2866,7 +2867,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>24</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>31</v>
       </c>
@@ -2948,7 +2949,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>31</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>31</v>
       </c>
@@ -3042,7 +3043,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>31</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>31</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>31</v>
       </c>

</xml_diff>